<commit_message>
updated yaml files and sources
</commit_message>
<xml_diff>
--- a/electricity/sources/Energetska bilanca, STAT.si in Podnebnik.xlsx
+++ b/electricity/sources/Energetska bilanca, STAT.si in Podnebnik.xlsx
@@ -752,7 +752,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1192,11 +1191,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223672320"/>
-        <c:axId val="178176576"/>
+        <c:axId val="118169600"/>
+        <c:axId val="224647360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="223672320"/>
+        <c:axId val="118169600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1238,7 +1237,7 @@
             <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178176576"/>
+        <c:crossAx val="224647360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1246,7 +1245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="178176576"/>
+        <c:axId val="224647360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1297,7 +1296,7 @@
             <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223672320"/>
+        <c:crossAx val="118169600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1339,7 +1338,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1491,11 +1489,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223672832"/>
-        <c:axId val="114299968"/>
+        <c:axId val="118171136"/>
+        <c:axId val="118235136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="223672832"/>
+        <c:axId val="118171136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1537,7 +1535,7 @@
             <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114299968"/>
+        <c:crossAx val="118235136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1545,7 +1543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114299968"/>
+        <c:axId val="118235136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1594,7 @@
             <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223672832"/>
+        <c:crossAx val="118171136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2468,11 +2466,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223858688"/>
-        <c:axId val="178180032"/>
+        <c:axId val="118172160"/>
+        <c:axId val="118237440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="223858688"/>
+        <c:axId val="118172160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2515,7 +2513,7 @@
             <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178180032"/>
+        <c:crossAx val="118237440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2523,7 +2521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="178180032"/>
+        <c:axId val="118237440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2574,7 +2572,7 @@
             <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223858688"/>
+        <c:crossAx val="118172160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2923,11 +2921,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="228291584"/>
-        <c:axId val="114353856"/>
+        <c:axId val="118173184"/>
+        <c:axId val="118240320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="228291584"/>
+        <c:axId val="118173184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2969,7 +2967,7 @@
             <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114353856"/>
+        <c:crossAx val="118240320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2977,7 +2975,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114353856"/>
+        <c:axId val="118240320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3028,7 +3026,7 @@
             <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228291584"/>
+        <c:crossAx val="118173184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6034,8 +6032,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="235248640"/>
-        <c:axId val="114355584"/>
+        <c:axId val="135439360"/>
+        <c:axId val="118242048"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6259,11 +6257,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="235248640"/>
-        <c:axId val="114355584"/>
+        <c:axId val="135439360"/>
+        <c:axId val="118242048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="235248640"/>
+        <c:axId val="135439360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6322,7 +6320,7 @@
             <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114355584"/>
+        <c:crossAx val="118242048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6330,7 +6328,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114355584"/>
+        <c:axId val="118242048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6397,7 +6395,7 @@
             <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235248640"/>
+        <c:crossAx val="135439360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12673,8 +12671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH12" sqref="AH12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12779,7 +12777,7 @@
       <c r="AF1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" s="36" t="s">
+      <c r="AG1" s="34" t="s">
         <v>78</v>
       </c>
       <c r="AH1" s="29" t="s">

</xml_diff>